<commit_message>
Did another few rounds of tests
Did some more tests with different plys then made the powerpoint and
paper parts for the results.
</commit_message>
<xml_diff>
--- a/final stats.xlsx
+++ b/final stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>A-B AI</t>
   </si>
@@ -55,6 +55,21 @@
   <si>
     <t>2 samp z-tests for p</t>
   </si>
+  <si>
+    <t>p-Values</t>
+  </si>
+  <si>
+    <t>A-B AI (4)</t>
+  </si>
+  <si>
+    <t>A-B AI (0)</t>
+  </si>
+  <si>
+    <t>A-B AI (10)</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
 </sst>
 </file>
 
@@ -69,15 +84,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +106,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,6 +147,1201 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Alpha-Beta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> versus Dumb AI</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dumb AI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sheriff</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Outlaws</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Renegade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$36:$M$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A-B AI (0)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sheriff</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Outlaws</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Renegade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$37:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A-B AI (4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sheriff</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Outlaws</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Renegade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$38:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A-B AI (10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sheriff</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Outlaws</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Renegade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$39:$M$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="43224360"/>
+        <c:axId val="43223968"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$J$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Expected</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$K$35:$M$35</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>Sheriff</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Outlaws</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Renegade</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$K$40:$M$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43224360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43223968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43223968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43224360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="I27" workbookViewId="0">
+      <selection activeCell="M35" sqref="J35:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C17">
         <v>1</v>
       </c>
@@ -527,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C18">
         <v>1</v>
       </c>
@@ -535,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>1</v>
       </c>
@@ -543,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1</v>
       </c>
@@ -551,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -559,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>1</v>
       </c>
@@ -567,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1</v>
       </c>
@@ -575,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C24">
         <v>1</v>
       </c>
@@ -583,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>1</v>
       </c>
@@ -591,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>1</v>
       </c>
@@ -599,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>1</v>
       </c>
@@ -607,55 +1843,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>1</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>1</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J29" s="2"/>
+      <c r="K29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>1</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.377</v>
+      </c>
+      <c r="L30" s="2">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="M30" s="2">
+        <v>8.1799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>1</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>1</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="2">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="L32" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="M32" s="2">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C33">
         <v>1</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="2">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="L33" s="2">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="M33" s="2">
+        <v>8.1799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>1</v>
       </c>
@@ -663,55 +1963,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C35">
         <v>1</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J35" s="2"/>
+      <c r="K35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>1</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>1</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>1</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="M38" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C41">
         <v>1</v>
       </c>
@@ -719,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>1</v>
       </c>
@@ -727,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>1</v>
       </c>
@@ -735,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>1</v>
       </c>
@@ -743,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>1</v>
       </c>
@@ -751,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>1</v>
       </c>
@@ -759,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C47">
         <v>1</v>
       </c>
@@ -767,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C48">
         <v>1</v>
       </c>
@@ -969,7 +2339,562 @@
         <v>1</v>
       </c>
     </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>2</v>
+      </c>
+      <c r="I66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <f>SUM(A67:C117)</f>
+        <v>100</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <f>SUM(G67:I117)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="I110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <f>SUM(A67:A116)</f>
+        <v>3</v>
+      </c>
+      <c r="B117">
+        <f>SUM(B67:B116)</f>
+        <v>42</v>
+      </c>
+      <c r="C117">
+        <f>SUM(C67:C116)</f>
+        <v>5</v>
+      </c>
+      <c r="G117">
+        <f>SUM(G67:G116)</f>
+        <v>8</v>
+      </c>
+      <c r="H117">
+        <f>SUM(H67:H116)</f>
+        <v>35</v>
+      </c>
+      <c r="I117">
+        <f>SUM(I67:I116)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <f>A117/50</f>
+        <v>0.06</v>
+      </c>
+      <c r="B118">
+        <f>B117/50</f>
+        <v>0.84</v>
+      </c>
+      <c r="C118">
+        <f>C117/50</f>
+        <v>0.1</v>
+      </c>
+      <c r="G118">
+        <f>G117/50</f>
+        <v>0.16</v>
+      </c>
+      <c r="H118">
+        <f>H117/50</f>
+        <v>0.7</v>
+      </c>
+      <c r="I118">
+        <f>I117/50</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>0.25</v>
+      </c>
+      <c r="B119">
+        <v>0.5</v>
+      </c>
+      <c r="C119">
+        <v>0.25</v>
+      </c>
+      <c r="G119">
+        <v>0.25</v>
+      </c>
+      <c r="H119">
+        <v>0.5</v>
+      </c>
+      <c r="I119">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <f>(A118-A119)/SQRT(A118*(1-A118)/$D$56)</f>
+        <v>-5.6571676746664306</v>
+      </c>
+      <c r="B121">
+        <f>(B118-B119)/SQRT(B118*(1-B118)/$D$56)</f>
+        <v>6.5578923733889054</v>
+      </c>
+      <c r="C121">
+        <f>(C118-C119)/SQRT(C118*(1-C118)/$D$56)</f>
+        <v>-3.5355339059327373</v>
+      </c>
+      <c r="G121">
+        <f>(G118-G119)/SQRT(G118*(1-G118)/$D$56)</f>
+        <v>-1.735912687073534</v>
+      </c>
+      <c r="H121">
+        <f>(H118-H119)/SQRT(H118*(1-H118)/$D$56)</f>
+        <v>3.086066999241837</v>
+      </c>
+      <c r="I121">
+        <f>(I118-I119)/SQRT(I118*(1-I118)/$D$56)</f>
+        <v>-2.241632651332861</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>0</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G122">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="H122">
+        <v>2E-3</v>
+      </c>
+      <c r="I122">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J28:M28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>